<commit_message>
add excel calc mock up
</commit_message>
<xml_diff>
--- a/data/Requested-PPDB-format.xlsx
+++ b/data/Requested-PPDB-format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\ghproj_CENTS\PLI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\PLIforDummies\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765AF0E8-CEEC-452E-8D5E-CE4328751BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F4202B-188C-4769-9572-B663B7E182CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21120" xr2:uid="{91A743A3-E3BB-4327-AD25-27565970C8D0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>substance</t>
   </si>
@@ -41,129 +41,9 @@
     <t>Birds.Acute.LD50.mg.kg</t>
   </si>
   <si>
-    <t>Reference.Value.Birds</t>
-  </si>
-  <si>
-    <t>Load.Factor.Birds</t>
-  </si>
-  <si>
-    <t>Mammals.Acute.Oral.LD50.mg.kg.BW.day</t>
-  </si>
-  <si>
-    <t>Reference.Value.Mammals</t>
-  </si>
-  <si>
-    <t>Load.Factor.Mammals</t>
-  </si>
-  <si>
-    <t>Fish.Acute.96hr.LC50.mg.l</t>
-  </si>
-  <si>
-    <t>Reference.Value.Fish</t>
-  </si>
-  <si>
-    <t>Load.Factor.Fish</t>
-  </si>
-  <si>
-    <t>Aquatic.Invertebrates.Acute.48hr.EC50.mg.l</t>
-  </si>
-  <si>
-    <t>Reference.Value.Aquatic.Invertebrates</t>
-  </si>
-  <si>
-    <t>Load.Factor.Aquatic.Invertebrates</t>
-  </si>
-  <si>
-    <t>Algae.Acute.72hr.EC50.Growth.mg.l</t>
-  </si>
-  <si>
-    <t>Reference.Value.Algae</t>
-  </si>
-  <si>
-    <t>Load.Factor.Algae</t>
-  </si>
-  <si>
-    <t>Aquatic.Plants.Acute.7d.EC50.mg.l</t>
-  </si>
-  <si>
-    <t>Reference.Value.Aquatic.Plants</t>
-  </si>
-  <si>
-    <t>Load.Factor.Aquatic.Plants</t>
-  </si>
-  <si>
     <t>Earthworms.Acute.14d.LC50.mg.kg</t>
   </si>
   <si>
-    <t>Reference.Value.Earthworms</t>
-  </si>
-  <si>
-    <t>Load.Factor.Earthworms</t>
-  </si>
-  <si>
-    <t>BeesLD50</t>
-  </si>
-  <si>
-    <t>Reference.Value.Bees</t>
-  </si>
-  <si>
-    <t>Load.Factor.Bees</t>
-  </si>
-  <si>
-    <t>Fish.Chronic.21d.NOEC.mg.l.corrected</t>
-  </si>
-  <si>
-    <t>Reference.Value.Fish.Chronic</t>
-  </si>
-  <si>
-    <t>Load.Factor.Fish.Chronic</t>
-  </si>
-  <si>
-    <t>water.phase.DT50.days</t>
-  </si>
-  <si>
-    <t>Aquatic.Invertebrates.Chronic.21d.NOEC.mg.l.correted</t>
-  </si>
-  <si>
-    <t>Reference.Value.Aquatic.Invertebrates.Chronic</t>
-  </si>
-  <si>
-    <t>Load.Factor.Aquatic.Invertebrates.Chronic</t>
-  </si>
-  <si>
-    <t>Earthworms.Chronic.14d.NOEC..Reproduction.mg.kg.corrected</t>
-  </si>
-  <si>
-    <t>Reference.Value.Earthworms.Chronic</t>
-  </si>
-  <si>
-    <t>Load.Factor.Earthworms.Chronic</t>
-  </si>
-  <si>
-    <t>2.1e-4</t>
-  </si>
-  <si>
-    <t>2.5e-5</t>
-  </si>
-  <si>
-    <t>3.6e-4</t>
-  </si>
-  <si>
-    <t>3.4</t>
-  </si>
-  <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>1.15e-4</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>Cyproconazol</t>
-  </si>
-  <si>
     <t>0.3777368</t>
   </si>
   <si>
@@ -176,68 +56,86 @@
     <t>0.65</t>
   </si>
   <si>
-    <t>0.29</t>
-  </si>
-  <si>
     <t>0.75</t>
   </si>
   <si>
-    <t>0.022</t>
-  </si>
-  <si>
-    <t>0.011</t>
-  </si>
-  <si>
-    <t>0.0053</t>
-  </si>
-  <si>
-    <t>1.93</t>
-  </si>
-  <si>
-    <t>0.008</t>
-  </si>
-  <si>
-    <t>1.1</t>
-  </si>
-  <si>
-    <t>0.003</t>
-  </si>
-  <si>
-    <t>3.5</t>
-  </si>
-  <si>
-    <t>watersedimentdt50_days</t>
-  </si>
-  <si>
-    <t>waterphasedt50_days</t>
-  </si>
-  <si>
-    <t>dt50typical_days</t>
-  </si>
-  <si>
-    <t>dt50field_days</t>
-  </si>
-  <si>
-    <t>casrn</t>
-  </si>
-  <si>
-    <t>pesticidetype</t>
-  </si>
-  <si>
-    <t>formulationapplicationdetails</t>
-  </si>
-  <si>
-    <t>scigrow</t>
-  </si>
-  <si>
-    <t>bcf_lkg</t>
+    <t>Cyproconazole</t>
+  </si>
+  <si>
+    <t>94361-06-5</t>
+  </si>
+  <si>
+    <t>fungicide</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>&lt;350</t>
+  </si>
+  <si>
+    <t>Honeybees.Contact.Acute.LD50.ug.bee</t>
+  </si>
+  <si>
+    <t>Temperate.Freshwater.Fish.Acute.96hr.LC50.mg.l</t>
+  </si>
+  <si>
+    <t>Temperate.Freshwater.Fish.Chronic.21d.NOEC.mg.l</t>
+  </si>
+  <si>
+    <t>Temperate.Freshwater.Aquatic.invertebrates.Acute.48hr.EC50.mg.l</t>
+  </si>
+  <si>
+    <t>Pesticide.type</t>
+  </si>
+  <si>
+    <t>CAS.RN</t>
+  </si>
+  <si>
+    <t>Soil.degradation.DT50.typical.days</t>
+  </si>
+  <si>
+    <t>Soil.degradation.DT50.field.days</t>
+  </si>
+  <si>
+    <t>Water.phase.only.DT50.days</t>
+  </si>
+  <si>
+    <t>SCIGROW.groundwater.index.ugl</t>
+  </si>
+  <si>
+    <t>Bioconcentration.factor.BCF.lkg</t>
+  </si>
+  <si>
+    <t>Mammals.Acute.oral.LD50.mg.kg</t>
+  </si>
+  <si>
+    <t>Earthworms.Chronic.NOEC.reproduction.mg.kg</t>
+  </si>
+  <si>
+    <t>&gt;100</t>
+  </si>
+  <si>
+    <t>&gt;22</t>
+  </si>
+  <si>
+    <t>Aquatic.plants.Acute.7d.EC50.mg.l</t>
+  </si>
+  <si>
+    <t>Algae.Acute.72hr.EC50.growth.mg.l</t>
+  </si>
+  <si>
+    <t>Temperate.Freshwater.Aquatic.invertebrates.Chronic.21d.NOEC.mgl</t>
+  </si>
+  <si>
+    <t>0.023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +269,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -714,9 +618,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1092,415 +1011,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FAA005-18EC-4A5C-8E7A-E9DB48E5CF15}">
-  <dimension ref="A1:AS3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="31" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="31" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="34.5546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="48.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="41.77734375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="38" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="56" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="58.88671875" customWidth="1"/>
+    <col min="18" max="18" width="31" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="K1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="L1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>142</v>
+      </c>
+      <c r="E2" s="3">
+        <v>129</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O1" t="s">
+      <c r="H2" s="3">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3">
+        <v>94</v>
+      </c>
+      <c r="K2" s="3">
+        <v>168</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="3">
+        <v>19</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" t="s">
-        <v>10</v>
-      </c>
-      <c r="V1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2">
-        <v>28</v>
-      </c>
-      <c r="L2">
-        <v>94</v>
-      </c>
-      <c r="M2">
-        <v>49</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>350</v>
-      </c>
-      <c r="P2">
-        <v>20</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>19</v>
-      </c>
-      <c r="S2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2">
-        <v>30</v>
-      </c>
-      <c r="U2">
-        <v>22</v>
-      </c>
-      <c r="V2" s="1">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="W2">
-        <v>30</v>
-      </c>
-      <c r="X2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2">
-        <v>3</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC2">
-        <v>3</v>
-      </c>
-      <c r="AD2">
-        <v>168</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF2">
-        <v>2</v>
-      </c>
-      <c r="AG2">
-        <v>100</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI2">
-        <v>100</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL2">
-        <v>3</v>
-      </c>
-      <c r="AM2">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP2">
-        <v>3</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="I3" s="1"/>
-      <c r="J3">
-        <v>431</v>
-      </c>
-      <c r="L3">
-        <v>2000</v>
-      </c>
-      <c r="M3">
-        <v>49</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>2000</v>
-      </c>
-      <c r="P3">
-        <v>20</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3">
-        <v>30</v>
-      </c>
-      <c r="U3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V3" s="1">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="W3">
-        <v>30</v>
-      </c>
-      <c r="X3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z3">
-        <v>3</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC3">
-        <v>3</v>
-      </c>
-      <c r="AD3">
-        <v>1000</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF3">
-        <v>2</v>
-      </c>
-      <c r="AG3">
-        <v>105</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI3">
-        <v>100</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL3">
-        <v>3</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP3">
-        <v>3</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS3">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>